<commit_message>
Collection details for those new samples
</commit_message>
<xml_diff>
--- a/backend/data-collections/Josh/Collection-details.xlsx
+++ b/backend/data-collections/Josh/Collection-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsummers/Library/CloudStorage/GoogleDrive-catalystjs@gmail.com/My Drive/Education/CS481/HandGestures/backend/data-collections/Josh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83423926-410F-4049-8ACE-3B7AD769FC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39B8701-0B8A-2043-B7D1-4E0CAB87557A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{4F85CC4F-1BCF-3A46-9CD3-A9F8342C348A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="101">
   <si>
     <t>Sample Number</t>
   </si>
@@ -255,6 +255,90 @@
   </si>
   <si>
     <t>Sitting/Laying</t>
+  </si>
+  <si>
+    <t>Josh24</t>
+  </si>
+  <si>
+    <t>Running</t>
+  </si>
+  <si>
+    <t>Josh25</t>
+  </si>
+  <si>
+    <t>Running, with hands at side, held down with minimal movement</t>
+  </si>
+  <si>
+    <t>Running (hands ar rest)</t>
+  </si>
+  <si>
+    <t>Running (hands active)</t>
+  </si>
+  <si>
+    <t>Josh26</t>
+  </si>
+  <si>
+    <t>Running, with hands pointing at objects</t>
+  </si>
+  <si>
+    <t>Josh27</t>
+  </si>
+  <si>
+    <t>Running, with hands in front of body, resting with hands on knees in middle</t>
+  </si>
+  <si>
+    <t>Running, with hands in front of body, held at angles (running position)</t>
+  </si>
+  <si>
+    <t>Josh28</t>
+  </si>
+  <si>
+    <t>Running, with hands in front of body, walking with hands at side halfway</t>
+  </si>
+  <si>
+    <t>Running/Walking</t>
+  </si>
+  <si>
+    <t>Josh29</t>
+  </si>
+  <si>
+    <t>Sitting in chair, hands on armrest, relaxing</t>
+  </si>
+  <si>
+    <t>Josh30</t>
+  </si>
+  <si>
+    <t>Sitting in chair, using mobile phone (swiping)</t>
+  </si>
+  <si>
+    <t>Sitting (hands active)</t>
+  </si>
+  <si>
+    <t>Josh31</t>
+  </si>
+  <si>
+    <t>Standing still, drinking a drink</t>
+  </si>
+  <si>
+    <t>Standing (hands active)</t>
+  </si>
+  <si>
+    <t>Josh32</t>
+  </si>
+  <si>
+    <t>Standing still, crouching to catch throw object (a few catches in sample)</t>
+  </si>
+  <si>
+    <t>Josh33</t>
+  </si>
+  <si>
+    <t>Walking upstairs and downstairs, jogging the steps (hands in front of body), but walking the flat surfaces</t>
+  </si>
+  <si>
+    <t>Josh34</t>
+  </si>
+  <si>
+    <t>Walking, drinking a drink and hands at side when not drinking (three sips were taken)</t>
   </si>
 </sst>
 </file>
@@ -626,16 +710,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DF80E3-7265-604C-BC16-95B756F6068B}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
@@ -1193,6 +1277,259 @@
         <v>31</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Another set of samples collected, along with their details
</commit_message>
<xml_diff>
--- a/backend/data-collections/Josh/Collection-details.xlsx
+++ b/backend/data-collections/Josh/Collection-details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsummers/Library/CloudStorage/GoogleDrive-catalystjs@gmail.com/My Drive/Education/CS481/HandGestures/backend/data-collections/Josh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39B8701-0B8A-2043-B7D1-4E0CAB87557A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261683E6-C43A-1243-9CB6-D93DA9407519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{4F85CC4F-1BCF-3A46-9CD3-A9F8342C348A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="155">
   <si>
     <t>Sample Number</t>
   </si>
@@ -339,6 +339,168 @@
   </si>
   <si>
     <t>Walking, drinking a drink and hands at side when not drinking (three sips were taken)</t>
+  </si>
+  <si>
+    <t>Josh35</t>
+  </si>
+  <si>
+    <t>Sitting at computer, using computer, then standing up and walking away half way through</t>
+  </si>
+  <si>
+    <t>Sitting/Walking</t>
+  </si>
+  <si>
+    <t>Josh36</t>
+  </si>
+  <si>
+    <t>Walking around room, collecting things, then sitting down at computer halfway and using computer</t>
+  </si>
+  <si>
+    <t>Walking/Sitting</t>
+  </si>
+  <si>
+    <t>Walking (hands active)</t>
+  </si>
+  <si>
+    <t>Josh37</t>
+  </si>
+  <si>
+    <t>Laying down, hands at rest on chest, then sitting up, hands at side at rest</t>
+  </si>
+  <si>
+    <t>Laying/Sitting</t>
+  </si>
+  <si>
+    <t>Josh38</t>
+  </si>
+  <si>
+    <t>Sitting down, using mobile phone (swiping), then standing up and using mobile phone (swiping)</t>
+  </si>
+  <si>
+    <t>Josh39</t>
+  </si>
+  <si>
+    <t>Laying down, using mobile phone (swiping), then standing up and walking while looking at phone (holding )</t>
+  </si>
+  <si>
+    <t>Laying/Walking</t>
+  </si>
+  <si>
+    <t>Laying (hands active)</t>
+  </si>
+  <si>
+    <t>Josh40</t>
+  </si>
+  <si>
+    <t>Sitting down, using computer when suddenly falling out of chair</t>
+  </si>
+  <si>
+    <t>Sitting/Falling</t>
+  </si>
+  <si>
+    <t>Josh41</t>
+  </si>
+  <si>
+    <t>Standing still, hands at side (at rest) when suddenly faillng to ground</t>
+  </si>
+  <si>
+    <t>Standing/Falling</t>
+  </si>
+  <si>
+    <t>Josh42</t>
+  </si>
+  <si>
+    <t>Walking hands at side, tripping and falling to ground</t>
+  </si>
+  <si>
+    <t>Walking/Falling</t>
+  </si>
+  <si>
+    <t>Josh43</t>
+  </si>
+  <si>
+    <t>Standing/Sitting</t>
+  </si>
+  <si>
+    <t>Josh44</t>
+  </si>
+  <si>
+    <t>Walking using mobile phone (swiping), then Laying down using mobile phoe (swiping) half way through</t>
+  </si>
+  <si>
+    <t>Standing using mobile phone (swiping), then sitting down in chair using mobile phone (swiping) half way through</t>
+  </si>
+  <si>
+    <t>Walking/Laying</t>
+  </si>
+  <si>
+    <t>Josh45</t>
+  </si>
+  <si>
+    <t>Walking using mobile phone (swiping), then stopping and standing still, which using mobile phone (swiping)</t>
+  </si>
+  <si>
+    <t>Walking/Standing</t>
+  </si>
+  <si>
+    <t>Josh46</t>
+  </si>
+  <si>
+    <t>Standing with hands at side (at rest), then sitting down in chair with hands on armsrests (at rest)</t>
+  </si>
+  <si>
+    <t>Standing with hands at side (at rest), then laying down on bed with hands on chest (at rest)</t>
+  </si>
+  <si>
+    <t>Standing/Laying</t>
+  </si>
+  <si>
+    <t>Josh47</t>
+  </si>
+  <si>
+    <t>Josh48</t>
+  </si>
+  <si>
+    <t>Standing using mobile phone (swiping), then laying down on bed using mobile phone (swiping) half way through</t>
+  </si>
+  <si>
+    <t>Josh49</t>
+  </si>
+  <si>
+    <t>Standing still talking, hands active (gesticulating) when suddenly falling to ground halfway through</t>
+  </si>
+  <si>
+    <t>Josh50</t>
+  </si>
+  <si>
+    <t>Laying down hands at side (at rest), then standing up and walking while hands at side (at rest)</t>
+  </si>
+  <si>
+    <t>Josh51</t>
+  </si>
+  <si>
+    <t>Walking around room hands at side (at rest), then sitting down at computer halfway with hands at rest</t>
+  </si>
+  <si>
+    <t>Josh52</t>
+  </si>
+  <si>
+    <t>Sitting at computer, using computer, then a subtle tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Tonic</t>
+  </si>
+  <si>
+    <t>Josh53</t>
+  </si>
+  <si>
+    <t>Sitting at computer, using computer, then a strong tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh54</t>
+  </si>
+  <si>
+    <t>Sitting at computer, using computer, then a extreme tonic condition occurs halfway through</t>
   </si>
 </sst>
 </file>
@@ -710,16 +872,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DF80E3-7265-604C-BC16-95B756F6068B}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="84.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
@@ -1245,7 +1407,7 @@
         <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
         <v>31</v>
@@ -1268,7 +1430,7 @@
         <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="F24" t="s">
         <v>31</v>
@@ -1383,7 +1545,7 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="F29" t="s">
         <v>78</v>
@@ -1528,6 +1690,466 @@
       </c>
       <c r="G35" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" t="s">
+        <v>91</v>
+      </c>
+      <c r="G39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" t="s">
+        <v>116</v>
+      </c>
+      <c r="G40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" t="s">
+        <v>66</v>
+      </c>
+      <c r="F43" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+      <c r="F44" t="s">
+        <v>94</v>
+      </c>
+      <c r="G44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" t="s">
+        <v>66</v>
+      </c>
+      <c r="F46" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" t="s">
+        <v>60</v>
+      </c>
+      <c r="G47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" t="s">
+        <v>66</v>
+      </c>
+      <c r="F48" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" t="s">
+        <v>94</v>
+      </c>
+      <c r="G49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" t="s">
+        <v>94</v>
+      </c>
+      <c r="G50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" t="s">
+        <v>115</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" t="s">
+        <v>66</v>
+      </c>
+      <c r="F51" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>146</v>
+      </c>
+      <c r="B52" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" t="s">
+        <v>33</v>
+      </c>
+      <c r="G52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="s">
+        <v>150</v>
+      </c>
+      <c r="F53" t="s">
+        <v>91</v>
+      </c>
+      <c r="G53" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" t="s">
+        <v>152</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" t="s">
+        <v>150</v>
+      </c>
+      <c r="F54" t="s">
+        <v>91</v>
+      </c>
+      <c r="G54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>153</v>
+      </c>
+      <c r="B55" t="s">
+        <v>154</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" t="s">
+        <v>150</v>
+      </c>
+      <c r="F55" t="s">
+        <v>91</v>
+      </c>
+      <c r="G55" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional data collection samples for Josh
</commit_message>
<xml_diff>
--- a/backend/data-collections/Josh/Collection-details.xlsx
+++ b/backend/data-collections/Josh/Collection-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsummers/Library/CloudStorage/GoogleDrive-catalystjs@gmail.com/My Drive/Education/CS481/HandGestures/backend/data-collections/Josh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261683E6-C43A-1243-9CB6-D93DA9407519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BCFF54-7CA6-E34F-A4B2-12C9B9AA1686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{4F85CC4F-1BCF-3A46-9CD3-A9F8342C348A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="283">
   <si>
     <t>Sample Number</t>
   </si>
@@ -501,6 +501,390 @@
   </si>
   <si>
     <t>Sitting at computer, using computer, then a extreme tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh55</t>
+  </si>
+  <si>
+    <t>Walking down stairs normally,then upstairs normally, and sitting down in chair right near the end</t>
+  </si>
+  <si>
+    <t>Josh56</t>
+  </si>
+  <si>
+    <t>Sitting at table, gesticulating with hands in conversation, then a subtle tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh57</t>
+  </si>
+  <si>
+    <t>Sitting at table, gesticulating with hands in conversation, then a strong tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Sitting at table, gesticulating with hands in conversation, then a extreme tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh58</t>
+  </si>
+  <si>
+    <t>Josh59</t>
+  </si>
+  <si>
+    <t>Standing still, hands at side (at rest), then a subtle tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh60</t>
+  </si>
+  <si>
+    <t>Standing still, hands at side (at rest), then a strong tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh61</t>
+  </si>
+  <si>
+    <t>Josh62</t>
+  </si>
+  <si>
+    <t>Standing still, hands at side (at rest), then a extreme tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Standing still using mobile phone (swiping), then a subtle tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh63</t>
+  </si>
+  <si>
+    <t>Standing still using mobile phone (swiping), then a strong tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh64</t>
+  </si>
+  <si>
+    <t>Standing still using mobile phone (swiping), then a extreme tonic condition occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh65</t>
+  </si>
+  <si>
+    <t>Walking around room hands at side (at rest), then stopping due to subtle tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh66</t>
+  </si>
+  <si>
+    <t>Walking around room hands at side (at rest), then slow walking due to subtle tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh67</t>
+  </si>
+  <si>
+    <t>Walking around room hands at side (at rest), then stopping due to strong tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh68</t>
+  </si>
+  <si>
+    <t>Walking around room hands at side (at rest), then stopping due to extreme tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh69</t>
+  </si>
+  <si>
+    <t>Walking around room using mobile phone (swiping), then stopping due to extreme tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Walking around room using mobile phone (swiping), then slow walking due to subtle tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh70</t>
+  </si>
+  <si>
+    <t>Walking around room using mobile phone (swiping), then stopping due to strong tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh71</t>
+  </si>
+  <si>
+    <t>Josh72</t>
+  </si>
+  <si>
+    <t>Walking around room using mobile phone (swiping), then stopping due to subtle tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh73</t>
+  </si>
+  <si>
+    <t>Walking outside hands at side (at rest), then stopping due to subtle tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh74</t>
+  </si>
+  <si>
+    <t>Walking outside hands at side (at rest), then stopping due to strong tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh75</t>
+  </si>
+  <si>
+    <t>Josh76</t>
+  </si>
+  <si>
+    <t>Josh77</t>
+  </si>
+  <si>
+    <t>Josh78</t>
+  </si>
+  <si>
+    <t>Josh79</t>
+  </si>
+  <si>
+    <t>Walking down the stairs, and then up the stairs, ultimately stopping still due to subtle tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Walking down the stairs, and then up the stairs, ultimately stopping still due to strong tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Walking down the stairs, and then up the stairs, ultimately stopping still due to extreme tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh80</t>
+  </si>
+  <si>
+    <t>Walking down the stairs slowly, and then walking until a strong tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Walking down the stairs slowly, and then walking until a subtle tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh81</t>
+  </si>
+  <si>
+    <t>Walking down the stairs slowly, and then walking until a extreme tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh82</t>
+  </si>
+  <si>
+    <t>Walking down the stairs slowly, using mobile phone (swiping), then a subtle tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Stairs (hands active)</t>
+  </si>
+  <si>
+    <t>Josh83</t>
+  </si>
+  <si>
+    <t>Walking down the stairs slowly, using mobile phone (swiping), then a strong tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Stairs (hands tonic)</t>
+  </si>
+  <si>
+    <t>Walking (hands tonic)</t>
+  </si>
+  <si>
+    <t>Sitting (hands tonic)</t>
+  </si>
+  <si>
+    <t>Standing (hands tonic)</t>
+  </si>
+  <si>
+    <t>Josh84</t>
+  </si>
+  <si>
+    <t>Walking down the stairs slowly, using mobile phone (swiping), then a extreme tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh85</t>
+  </si>
+  <si>
+    <t>Walking outside using mobile phone (swiping), then stopping due to subtle tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Walking outside using mobile phone (swiping), then stopping due to strong tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Walking outside using mobile phone (swiping), then stopping due to extreme tonic episode halfway through</t>
+  </si>
+  <si>
+    <t>Josh86</t>
+  </si>
+  <si>
+    <t>Josh87</t>
+  </si>
+  <si>
+    <t>Josh88</t>
+  </si>
+  <si>
+    <t>Josh89</t>
+  </si>
+  <si>
+    <t>Josh90</t>
+  </si>
+  <si>
+    <t>Josh91</t>
+  </si>
+  <si>
+    <t>Sitting at table, gesticulating with hands in conversation, then a subtle tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Sitting at computer, using computer,  then a strong tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Sitting at computer, using computer,  then a subtle tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Tremor</t>
+  </si>
+  <si>
+    <t>Sitting (hands tremor)</t>
+  </si>
+  <si>
+    <t>Josh92</t>
+  </si>
+  <si>
+    <t>Sitting at table, gesticulating with hands in conversation, then a strong tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Josh93</t>
+  </si>
+  <si>
+    <t>Josh94</t>
+  </si>
+  <si>
+    <t>Sitting at table, drinking a drink, when a subtle tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Josh95</t>
+  </si>
+  <si>
+    <t>Josh96</t>
+  </si>
+  <si>
+    <t>Josh97</t>
+  </si>
+  <si>
+    <t>Sitting at table, using mobile phone (swiping), when a subtle tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Sitting at table, drinking a drink, when a strong tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Josh98</t>
+  </si>
+  <si>
+    <t>Josh99</t>
+  </si>
+  <si>
+    <t>Sitting at table, using mobile phone (swiping), when a strong tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Josh100</t>
+  </si>
+  <si>
+    <t>Standing still, hands at side (at rest), then a subtle tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Standing (hands tremor)</t>
+  </si>
+  <si>
+    <t>Josh101</t>
+  </si>
+  <si>
+    <t>Josh102</t>
+  </si>
+  <si>
+    <t>Standing still, hands at side (at rest), then a strong tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Josh103</t>
+  </si>
+  <si>
+    <t>Standing still talking, hands active (gesticulating) when a subtle tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Standing still, hands at side (at rest), then an extreme tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Sitting at table, using mobile phone (swiping), when an extreme tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Sitting at table, drinking a drink, when an extreme tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Sitting at table, gesticulating with hands in conversation, then an extreme tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Sitting at computer, using computer, then an extreme tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Josh104</t>
+  </si>
+  <si>
+    <t>Josh105</t>
+  </si>
+  <si>
+    <t>Standing still talking, hands active (gesticulating) when a strong tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Standing still talking, hands active (gesticulating) when an extreme tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Josh106</t>
+  </si>
+  <si>
+    <t>Standing still using mobile phone (swiping), when an subtle tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Standing still using mobile phone (swiping), when an strong tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Standing still using mobile phone (swiping), when an extreme tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Josh107</t>
+  </si>
+  <si>
+    <t>Josh108</t>
+  </si>
+  <si>
+    <t>Josh109</t>
+  </si>
+  <si>
+    <t>Josh110</t>
+  </si>
+  <si>
+    <t>Josh111</t>
+  </si>
+  <si>
+    <t>Walking around room hands at side (at rest), when an subtle tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Walking around room hands at side (at rest), when an strong tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Walking around room hands at side (at rest), when an extreme tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Walking (hands tremor)</t>
+  </si>
+  <si>
+    <t>Josh112</t>
+  </si>
+  <si>
+    <t>Walking around room using mobile phone (swiping), then stopping due a subtle tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Josh113</t>
+  </si>
+  <si>
+    <t>Josh114</t>
+  </si>
+  <si>
+    <t>Walking around room using mobile phone (swiping), then stopping due a strong tonic and tremor episode occurs quarter way through</t>
+  </si>
+  <si>
+    <t>Walking around room using mobile phone (swiping), then stopping due a extreme tonic and tremor episode occurs quarter way through</t>
   </si>
 </sst>
 </file>
@@ -872,16 +1256,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DF80E3-7265-604C-BC16-95B756F6068B}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55:G55"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="91.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="108.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
@@ -2152,6 +2536,1386 @@
         <v>31</v>
       </c>
     </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" t="s">
+        <v>66</v>
+      </c>
+      <c r="F56" t="s">
+        <v>33</v>
+      </c>
+      <c r="G56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>157</v>
+      </c>
+      <c r="B57" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" t="s">
+        <v>150</v>
+      </c>
+      <c r="F57" t="s">
+        <v>91</v>
+      </c>
+      <c r="G57" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>159</v>
+      </c>
+      <c r="B58" t="s">
+        <v>160</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" t="s">
+        <v>150</v>
+      </c>
+      <c r="F58" t="s">
+        <v>91</v>
+      </c>
+      <c r="G58" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>162</v>
+      </c>
+      <c r="B59" t="s">
+        <v>161</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" t="s">
+        <v>150</v>
+      </c>
+      <c r="F59" t="s">
+        <v>91</v>
+      </c>
+      <c r="G59" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>163</v>
+      </c>
+      <c r="B60" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" t="s">
+        <v>150</v>
+      </c>
+      <c r="F60" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>165</v>
+      </c>
+      <c r="B61" t="s">
+        <v>166</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" t="s">
+        <v>150</v>
+      </c>
+      <c r="F61" t="s">
+        <v>32</v>
+      </c>
+      <c r="G61" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>167</v>
+      </c>
+      <c r="B62" t="s">
+        <v>169</v>
+      </c>
+      <c r="C62" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" t="s">
+        <v>150</v>
+      </c>
+      <c r="F62" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63" t="s">
+        <v>150</v>
+      </c>
+      <c r="F63" t="s">
+        <v>94</v>
+      </c>
+      <c r="G63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>171</v>
+      </c>
+      <c r="B64" t="s">
+        <v>172</v>
+      </c>
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" t="s">
+        <v>150</v>
+      </c>
+      <c r="F64" t="s">
+        <v>94</v>
+      </c>
+      <c r="G64" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>173</v>
+      </c>
+      <c r="B65" t="s">
+        <v>174</v>
+      </c>
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" t="s">
+        <v>150</v>
+      </c>
+      <c r="F65" t="s">
+        <v>94</v>
+      </c>
+      <c r="G65" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>175</v>
+      </c>
+      <c r="B66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" t="s">
+        <v>150</v>
+      </c>
+      <c r="F66" t="s">
+        <v>33</v>
+      </c>
+      <c r="G66" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>177</v>
+      </c>
+      <c r="B67" t="s">
+        <v>178</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" t="s">
+        <v>150</v>
+      </c>
+      <c r="F67" t="s">
+        <v>33</v>
+      </c>
+      <c r="G67" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>179</v>
+      </c>
+      <c r="B68" t="s">
+        <v>180</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" t="s">
+        <v>150</v>
+      </c>
+      <c r="F68" t="s">
+        <v>33</v>
+      </c>
+      <c r="G68" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" t="s">
+        <v>182</v>
+      </c>
+      <c r="C69" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>150</v>
+      </c>
+      <c r="F69" t="s">
+        <v>33</v>
+      </c>
+      <c r="G69" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>183</v>
+      </c>
+      <c r="B70" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" t="s">
+        <v>150</v>
+      </c>
+      <c r="F70" t="s">
+        <v>107</v>
+      </c>
+      <c r="G70" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>186</v>
+      </c>
+      <c r="B71" t="s">
+        <v>187</v>
+      </c>
+      <c r="C71" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" t="s">
+        <v>150</v>
+      </c>
+      <c r="F71" t="s">
+        <v>107</v>
+      </c>
+      <c r="G71" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>188</v>
+      </c>
+      <c r="B72" t="s">
+        <v>184</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" t="s">
+        <v>150</v>
+      </c>
+      <c r="F72" t="s">
+        <v>107</v>
+      </c>
+      <c r="G72" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>189</v>
+      </c>
+      <c r="B73" t="s">
+        <v>190</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" t="s">
+        <v>150</v>
+      </c>
+      <c r="F73" t="s">
+        <v>107</v>
+      </c>
+      <c r="G73" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>191</v>
+      </c>
+      <c r="B74" t="s">
+        <v>192</v>
+      </c>
+      <c r="C74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" t="s">
+        <v>150</v>
+      </c>
+      <c r="F74" t="s">
+        <v>33</v>
+      </c>
+      <c r="G74" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75" t="s">
+        <v>194</v>
+      </c>
+      <c r="C75" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" t="s">
+        <v>150</v>
+      </c>
+      <c r="F75" t="s">
+        <v>33</v>
+      </c>
+      <c r="G75" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>195</v>
+      </c>
+      <c r="B76" t="s">
+        <v>194</v>
+      </c>
+      <c r="C76" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" t="s">
+        <v>150</v>
+      </c>
+      <c r="F76" t="s">
+        <v>33</v>
+      </c>
+      <c r="G76" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>196</v>
+      </c>
+      <c r="B77" t="s">
+        <v>200</v>
+      </c>
+      <c r="C77" t="s">
+        <v>59</v>
+      </c>
+      <c r="D77" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" t="s">
+        <v>150</v>
+      </c>
+      <c r="F77" t="s">
+        <v>60</v>
+      </c>
+      <c r="G77" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>197</v>
+      </c>
+      <c r="B78" t="s">
+        <v>201</v>
+      </c>
+      <c r="C78" t="s">
+        <v>59</v>
+      </c>
+      <c r="D78" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" t="s">
+        <v>150</v>
+      </c>
+      <c r="F78" t="s">
+        <v>60</v>
+      </c>
+      <c r="G78" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>198</v>
+      </c>
+      <c r="B79" t="s">
+        <v>202</v>
+      </c>
+      <c r="C79" t="s">
+        <v>59</v>
+      </c>
+      <c r="D79" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" t="s">
+        <v>150</v>
+      </c>
+      <c r="F79" t="s">
+        <v>60</v>
+      </c>
+      <c r="G79" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>199</v>
+      </c>
+      <c r="B80" t="s">
+        <v>205</v>
+      </c>
+      <c r="C80" t="s">
+        <v>59</v>
+      </c>
+      <c r="D80" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" t="s">
+        <v>150</v>
+      </c>
+      <c r="F80" t="s">
+        <v>60</v>
+      </c>
+      <c r="G80" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>203</v>
+      </c>
+      <c r="B81" t="s">
+        <v>204</v>
+      </c>
+      <c r="C81" t="s">
+        <v>59</v>
+      </c>
+      <c r="D81" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" t="s">
+        <v>150</v>
+      </c>
+      <c r="F81" t="s">
+        <v>60</v>
+      </c>
+      <c r="G81" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>206</v>
+      </c>
+      <c r="B82" t="s">
+        <v>207</v>
+      </c>
+      <c r="C82" t="s">
+        <v>59</v>
+      </c>
+      <c r="D82" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" t="s">
+        <v>150</v>
+      </c>
+      <c r="F82" t="s">
+        <v>60</v>
+      </c>
+      <c r="G82" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>208</v>
+      </c>
+      <c r="B83" t="s">
+        <v>209</v>
+      </c>
+      <c r="C83" t="s">
+        <v>59</v>
+      </c>
+      <c r="D83" t="s">
+        <v>28</v>
+      </c>
+      <c r="E83" t="s">
+        <v>150</v>
+      </c>
+      <c r="F83" t="s">
+        <v>210</v>
+      </c>
+      <c r="G83" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>211</v>
+      </c>
+      <c r="B84" t="s">
+        <v>212</v>
+      </c>
+      <c r="C84" t="s">
+        <v>59</v>
+      </c>
+      <c r="D84" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" t="s">
+        <v>150</v>
+      </c>
+      <c r="F84" t="s">
+        <v>210</v>
+      </c>
+      <c r="G84" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>217</v>
+      </c>
+      <c r="B85" t="s">
+        <v>218</v>
+      </c>
+      <c r="C85" t="s">
+        <v>59</v>
+      </c>
+      <c r="D85" t="s">
+        <v>28</v>
+      </c>
+      <c r="E85" t="s">
+        <v>150</v>
+      </c>
+      <c r="F85" t="s">
+        <v>210</v>
+      </c>
+      <c r="G85" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>219</v>
+      </c>
+      <c r="B86" t="s">
+        <v>220</v>
+      </c>
+      <c r="C86" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86" t="s">
+        <v>28</v>
+      </c>
+      <c r="E86" t="s">
+        <v>150</v>
+      </c>
+      <c r="F86" t="s">
+        <v>107</v>
+      </c>
+      <c r="G86" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>223</v>
+      </c>
+      <c r="B87" t="s">
+        <v>221</v>
+      </c>
+      <c r="C87" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" t="s">
+        <v>28</v>
+      </c>
+      <c r="E87" t="s">
+        <v>150</v>
+      </c>
+      <c r="F87" t="s">
+        <v>107</v>
+      </c>
+      <c r="G87" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>224</v>
+      </c>
+      <c r="B88" t="s">
+        <v>222</v>
+      </c>
+      <c r="C88" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" t="s">
+        <v>150</v>
+      </c>
+      <c r="F88" t="s">
+        <v>107</v>
+      </c>
+      <c r="G88" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>225</v>
+      </c>
+      <c r="B89" t="s">
+        <v>231</v>
+      </c>
+      <c r="C89" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" t="s">
+        <v>28</v>
+      </c>
+      <c r="E89" t="s">
+        <v>232</v>
+      </c>
+      <c r="F89" t="s">
+        <v>91</v>
+      </c>
+      <c r="G89" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>226</v>
+      </c>
+      <c r="B90" t="s">
+        <v>230</v>
+      </c>
+      <c r="C90" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" t="s">
+        <v>28</v>
+      </c>
+      <c r="E90" t="s">
+        <v>232</v>
+      </c>
+      <c r="F90" t="s">
+        <v>91</v>
+      </c>
+      <c r="G90" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>227</v>
+      </c>
+      <c r="B91" t="s">
+        <v>259</v>
+      </c>
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" t="s">
+        <v>28</v>
+      </c>
+      <c r="E91" t="s">
+        <v>232</v>
+      </c>
+      <c r="F91" t="s">
+        <v>91</v>
+      </c>
+      <c r="G91" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>228</v>
+      </c>
+      <c r="B92" t="s">
+        <v>229</v>
+      </c>
+      <c r="C92" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" t="s">
+        <v>232</v>
+      </c>
+      <c r="F92" t="s">
+        <v>91</v>
+      </c>
+      <c r="G92" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>234</v>
+      </c>
+      <c r="B93" t="s">
+        <v>235</v>
+      </c>
+      <c r="C93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" t="s">
+        <v>28</v>
+      </c>
+      <c r="E93" t="s">
+        <v>232</v>
+      </c>
+      <c r="F93" t="s">
+        <v>91</v>
+      </c>
+      <c r="G93" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>236</v>
+      </c>
+      <c r="B94" t="s">
+        <v>258</v>
+      </c>
+      <c r="C94" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" t="s">
+        <v>232</v>
+      </c>
+      <c r="F94" t="s">
+        <v>91</v>
+      </c>
+      <c r="G94" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>237</v>
+      </c>
+      <c r="B95" t="s">
+        <v>238</v>
+      </c>
+      <c r="C95" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" t="s">
+        <v>28</v>
+      </c>
+      <c r="E95" t="s">
+        <v>232</v>
+      </c>
+      <c r="F95" t="s">
+        <v>31</v>
+      </c>
+      <c r="G95" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>239</v>
+      </c>
+      <c r="B96" t="s">
+        <v>243</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" t="s">
+        <v>28</v>
+      </c>
+      <c r="E96" t="s">
+        <v>232</v>
+      </c>
+      <c r="F96" t="s">
+        <v>31</v>
+      </c>
+      <c r="G96" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>240</v>
+      </c>
+      <c r="B97" t="s">
+        <v>257</v>
+      </c>
+      <c r="C97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" t="s">
+        <v>28</v>
+      </c>
+      <c r="E97" t="s">
+        <v>232</v>
+      </c>
+      <c r="F97" t="s">
+        <v>31</v>
+      </c>
+      <c r="G97" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>241</v>
+      </c>
+      <c r="B98" t="s">
+        <v>242</v>
+      </c>
+      <c r="C98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" t="s">
+        <v>28</v>
+      </c>
+      <c r="E98" t="s">
+        <v>232</v>
+      </c>
+      <c r="F98" t="s">
+        <v>91</v>
+      </c>
+      <c r="G98" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>244</v>
+      </c>
+      <c r="B99" t="s">
+        <v>246</v>
+      </c>
+      <c r="C99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" t="s">
+        <v>28</v>
+      </c>
+      <c r="E99" t="s">
+        <v>232</v>
+      </c>
+      <c r="F99" t="s">
+        <v>91</v>
+      </c>
+      <c r="G99" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>245</v>
+      </c>
+      <c r="B100" t="s">
+        <v>256</v>
+      </c>
+      <c r="C100" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" t="s">
+        <v>28</v>
+      </c>
+      <c r="E100" t="s">
+        <v>232</v>
+      </c>
+      <c r="F100" t="s">
+        <v>91</v>
+      </c>
+      <c r="G100" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>247</v>
+      </c>
+      <c r="B101" t="s">
+        <v>248</v>
+      </c>
+      <c r="C101" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" t="s">
+        <v>10</v>
+      </c>
+      <c r="E101" t="s">
+        <v>232</v>
+      </c>
+      <c r="F101" t="s">
+        <v>32</v>
+      </c>
+      <c r="G101" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>250</v>
+      </c>
+      <c r="B102" t="s">
+        <v>252</v>
+      </c>
+      <c r="C102" t="s">
+        <v>13</v>
+      </c>
+      <c r="D102" t="s">
+        <v>10</v>
+      </c>
+      <c r="E102" t="s">
+        <v>232</v>
+      </c>
+      <c r="F102" t="s">
+        <v>32</v>
+      </c>
+      <c r="G102" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>251</v>
+      </c>
+      <c r="B103" t="s">
+        <v>255</v>
+      </c>
+      <c r="C103" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" t="s">
+        <v>232</v>
+      </c>
+      <c r="F103" t="s">
+        <v>32</v>
+      </c>
+      <c r="G103" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>253</v>
+      </c>
+      <c r="B104" t="s">
+        <v>254</v>
+      </c>
+      <c r="C104" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104" t="s">
+        <v>28</v>
+      </c>
+      <c r="E104" t="s">
+        <v>232</v>
+      </c>
+      <c r="F104" t="s">
+        <v>94</v>
+      </c>
+      <c r="G104" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>260</v>
+      </c>
+      <c r="B105" t="s">
+        <v>262</v>
+      </c>
+      <c r="C105" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105" t="s">
+        <v>28</v>
+      </c>
+      <c r="E105" t="s">
+        <v>232</v>
+      </c>
+      <c r="F105" t="s">
+        <v>94</v>
+      </c>
+      <c r="G105" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>261</v>
+      </c>
+      <c r="B106" t="s">
+        <v>263</v>
+      </c>
+      <c r="C106" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" t="s">
+        <v>28</v>
+      </c>
+      <c r="E106" t="s">
+        <v>232</v>
+      </c>
+      <c r="F106" t="s">
+        <v>94</v>
+      </c>
+      <c r="G106" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>264</v>
+      </c>
+      <c r="B107" t="s">
+        <v>265</v>
+      </c>
+      <c r="C107" t="s">
+        <v>13</v>
+      </c>
+      <c r="D107" t="s">
+        <v>28</v>
+      </c>
+      <c r="E107" t="s">
+        <v>232</v>
+      </c>
+      <c r="F107" t="s">
+        <v>94</v>
+      </c>
+      <c r="G107" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>268</v>
+      </c>
+      <c r="B108" t="s">
+        <v>266</v>
+      </c>
+      <c r="C108" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108" t="s">
+        <v>28</v>
+      </c>
+      <c r="E108" t="s">
+        <v>232</v>
+      </c>
+      <c r="F108" t="s">
+        <v>94</v>
+      </c>
+      <c r="G108" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>269</v>
+      </c>
+      <c r="B109" t="s">
+        <v>267</v>
+      </c>
+      <c r="C109" t="s">
+        <v>13</v>
+      </c>
+      <c r="D109" t="s">
+        <v>28</v>
+      </c>
+      <c r="E109" t="s">
+        <v>232</v>
+      </c>
+      <c r="F109" t="s">
+        <v>94</v>
+      </c>
+      <c r="G109" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>270</v>
+      </c>
+      <c r="B110" t="s">
+        <v>273</v>
+      </c>
+      <c r="C110" t="s">
+        <v>18</v>
+      </c>
+      <c r="D110" t="s">
+        <v>10</v>
+      </c>
+      <c r="E110" t="s">
+        <v>232</v>
+      </c>
+      <c r="F110" t="s">
+        <v>33</v>
+      </c>
+      <c r="G110" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>271</v>
+      </c>
+      <c r="B111" t="s">
+        <v>274</v>
+      </c>
+      <c r="C111" t="s">
+        <v>18</v>
+      </c>
+      <c r="D111" t="s">
+        <v>10</v>
+      </c>
+      <c r="E111" t="s">
+        <v>232</v>
+      </c>
+      <c r="F111" t="s">
+        <v>33</v>
+      </c>
+      <c r="G111" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>272</v>
+      </c>
+      <c r="B112" t="s">
+        <v>275</v>
+      </c>
+      <c r="C112" t="s">
+        <v>18</v>
+      </c>
+      <c r="D112" t="s">
+        <v>10</v>
+      </c>
+      <c r="E112" t="s">
+        <v>232</v>
+      </c>
+      <c r="F112" t="s">
+        <v>33</v>
+      </c>
+      <c r="G112" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>277</v>
+      </c>
+      <c r="B113" t="s">
+        <v>278</v>
+      </c>
+      <c r="C113" t="s">
+        <v>18</v>
+      </c>
+      <c r="D113" t="s">
+        <v>28</v>
+      </c>
+      <c r="E113" t="s">
+        <v>232</v>
+      </c>
+      <c r="F113" t="s">
+        <v>107</v>
+      </c>
+      <c r="G113" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>279</v>
+      </c>
+      <c r="B114" t="s">
+        <v>281</v>
+      </c>
+      <c r="C114" t="s">
+        <v>18</v>
+      </c>
+      <c r="D114" t="s">
+        <v>28</v>
+      </c>
+      <c r="E114" t="s">
+        <v>232</v>
+      </c>
+      <c r="F114" t="s">
+        <v>107</v>
+      </c>
+      <c r="G114" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>280</v>
+      </c>
+      <c r="B115" t="s">
+        <v>282</v>
+      </c>
+      <c r="C115" t="s">
+        <v>18</v>
+      </c>
+      <c r="D115" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115" t="s">
+        <v>232</v>
+      </c>
+      <c r="F115" t="s">
+        <v>107</v>
+      </c>
+      <c r="G115" t="s">
+        <v>276</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Final data collecton files and variant count: reconciled duplicates and file structure
</commit_message>
<xml_diff>
--- a/backend/data-collections/Josh/Collection-details.xlsx
+++ b/backend/data-collections/Josh/Collection-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsummers/Library/CloudStorage/GoogleDrive-catalystjs@gmail.com/My Drive/Education/CS481/HandGestures/backend/data-collections/Josh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1376F3-4F84-B64E-93FD-1870E0452AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A03600-5C37-AB46-8C59-73B7EA975A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{4F85CC4F-1BCF-3A46-9CD3-A9F8342C348A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="374">
   <si>
     <t>Sample Number</t>
   </si>
@@ -1020,6 +1020,144 @@
   </si>
   <si>
     <t>Josh135</t>
+  </si>
+  <si>
+    <t>Josh136</t>
+  </si>
+  <si>
+    <t>Laying down, hands at rest on chest, when a subtle tonic and tremor episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying (hands tremor)</t>
+  </si>
+  <si>
+    <t>Laying down, hands at rest on chest, when a strong tonic and tremor episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying down, hands at rest on chest, when a extreme tonic and tremor episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh137</t>
+  </si>
+  <si>
+    <t>Josh138</t>
+  </si>
+  <si>
+    <t>Laying down, using mobile phone (swiping), when a subtle tonic and tremor episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh139</t>
+  </si>
+  <si>
+    <t>Josh140</t>
+  </si>
+  <si>
+    <t>Josh141</t>
+  </si>
+  <si>
+    <t>Laying down, using remote and watching TV, when a subtle tonic and tremor episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh142</t>
+  </si>
+  <si>
+    <t>Josh143</t>
+  </si>
+  <si>
+    <t>Josh144</t>
+  </si>
+  <si>
+    <t>Laying down, hands at rest on chest, when a subtle tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying down, hands at rest on chest, when a strong tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying down, hands at rest on chest, when a extreme tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying down, using mobile phone (swiping), when a subtle tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying down, using remote and watching TV, when a subtle tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying down, using mobile phone (swiping), when a strong tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying down, using mobile phone (swiping), when a extreme tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying down, using remote and watching TV, when a strong tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying down, using remote and watching TV, when a extreme tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Laying (hands tonic)</t>
+  </si>
+  <si>
+    <t>Josh145</t>
+  </si>
+  <si>
+    <t>Josh146</t>
+  </si>
+  <si>
+    <t>Josh147</t>
+  </si>
+  <si>
+    <t>Josh148</t>
+  </si>
+  <si>
+    <t>Josh149</t>
+  </si>
+  <si>
+    <t>Josh150</t>
+  </si>
+  <si>
+    <t>Josh151</t>
+  </si>
+  <si>
+    <t>Josh152</t>
+  </si>
+  <si>
+    <t>Josh153</t>
+  </si>
+  <si>
+    <t>Josh154</t>
+  </si>
+  <si>
+    <t>Josh155</t>
+  </si>
+  <si>
+    <t>Running down the street, hands at side swinging, and then stopping when a subtle tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Running down the street, hands at side swinging, and then stopping when a strong tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Running down the street, hands at side swinging, and then stopping when a extreme tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh156</t>
+  </si>
+  <si>
+    <t>Running down the street, hands held down at sides (minimal movement), and then stopping when a subtle tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Running down the street, hands held down at sides (minimal movement), and then stopping when a strong tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Running down the street, hands held down at sides (minimal movement), and then stopping when a extreme tonic episode occurs halfway through</t>
+  </si>
+  <si>
+    <t>Josh157</t>
+  </si>
+  <si>
+    <t>Josh159</t>
+  </si>
+  <si>
+    <t>Josh158</t>
   </si>
 </sst>
 </file>
@@ -1391,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DF80E3-7265-604C-BC16-95B756F6068B}">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4534,6 +4672,558 @@
         <v>316</v>
       </c>
     </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>328</v>
+      </c>
+      <c r="B137" t="s">
+        <v>329</v>
+      </c>
+      <c r="C137" t="s">
+        <v>27</v>
+      </c>
+      <c r="D137" t="s">
+        <v>19</v>
+      </c>
+      <c r="E137" t="s">
+        <v>232</v>
+      </c>
+      <c r="F137" t="s">
+        <v>34</v>
+      </c>
+      <c r="G137" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>333</v>
+      </c>
+      <c r="B138" t="s">
+        <v>331</v>
+      </c>
+      <c r="C138" t="s">
+        <v>27</v>
+      </c>
+      <c r="D138" t="s">
+        <v>19</v>
+      </c>
+      <c r="E138" t="s">
+        <v>232</v>
+      </c>
+      <c r="F138" t="s">
+        <v>34</v>
+      </c>
+      <c r="G138" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>334</v>
+      </c>
+      <c r="B139" t="s">
+        <v>332</v>
+      </c>
+      <c r="C139" t="s">
+        <v>27</v>
+      </c>
+      <c r="D139" t="s">
+        <v>19</v>
+      </c>
+      <c r="E139" t="s">
+        <v>232</v>
+      </c>
+      <c r="F139" t="s">
+        <v>34</v>
+      </c>
+      <c r="G139" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>336</v>
+      </c>
+      <c r="B140" t="s">
+        <v>335</v>
+      </c>
+      <c r="C140" t="s">
+        <v>27</v>
+      </c>
+      <c r="D140" t="s">
+        <v>28</v>
+      </c>
+      <c r="E140" t="s">
+        <v>232</v>
+      </c>
+      <c r="F140" t="s">
+        <v>116</v>
+      </c>
+      <c r="G140" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>337</v>
+      </c>
+      <c r="B141" t="s">
+        <v>335</v>
+      </c>
+      <c r="C141" t="s">
+        <v>27</v>
+      </c>
+      <c r="D141" t="s">
+        <v>28</v>
+      </c>
+      <c r="E141" t="s">
+        <v>232</v>
+      </c>
+      <c r="F141" t="s">
+        <v>116</v>
+      </c>
+      <c r="G141" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>338</v>
+      </c>
+      <c r="B142" t="s">
+        <v>335</v>
+      </c>
+      <c r="C142" t="s">
+        <v>27</v>
+      </c>
+      <c r="D142" t="s">
+        <v>28</v>
+      </c>
+      <c r="E142" t="s">
+        <v>232</v>
+      </c>
+      <c r="F142" t="s">
+        <v>116</v>
+      </c>
+      <c r="G142" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>340</v>
+      </c>
+      <c r="B143" t="s">
+        <v>339</v>
+      </c>
+      <c r="C143" t="s">
+        <v>27</v>
+      </c>
+      <c r="D143" t="s">
+        <v>28</v>
+      </c>
+      <c r="E143" t="s">
+        <v>232</v>
+      </c>
+      <c r="F143" t="s">
+        <v>116</v>
+      </c>
+      <c r="G143" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>341</v>
+      </c>
+      <c r="B144" t="s">
+        <v>339</v>
+      </c>
+      <c r="C144" t="s">
+        <v>27</v>
+      </c>
+      <c r="D144" t="s">
+        <v>28</v>
+      </c>
+      <c r="E144" t="s">
+        <v>232</v>
+      </c>
+      <c r="F144" t="s">
+        <v>116</v>
+      </c>
+      <c r="G144" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>342</v>
+      </c>
+      <c r="B145" t="s">
+        <v>339</v>
+      </c>
+      <c r="C145" t="s">
+        <v>27</v>
+      </c>
+      <c r="D145" t="s">
+        <v>28</v>
+      </c>
+      <c r="E145" t="s">
+        <v>232</v>
+      </c>
+      <c r="F145" t="s">
+        <v>116</v>
+      </c>
+      <c r="G145" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>353</v>
+      </c>
+      <c r="B146" t="s">
+        <v>343</v>
+      </c>
+      <c r="C146" t="s">
+        <v>27</v>
+      </c>
+      <c r="D146" t="s">
+        <v>19</v>
+      </c>
+      <c r="E146" t="s">
+        <v>150</v>
+      </c>
+      <c r="F146" t="s">
+        <v>34</v>
+      </c>
+      <c r="G146" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>354</v>
+      </c>
+      <c r="B147" t="s">
+        <v>344</v>
+      </c>
+      <c r="C147" t="s">
+        <v>27</v>
+      </c>
+      <c r="D147" t="s">
+        <v>19</v>
+      </c>
+      <c r="E147" t="s">
+        <v>150</v>
+      </c>
+      <c r="F147" t="s">
+        <v>34</v>
+      </c>
+      <c r="G147" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>355</v>
+      </c>
+      <c r="B148" t="s">
+        <v>345</v>
+      </c>
+      <c r="C148" t="s">
+        <v>27</v>
+      </c>
+      <c r="D148" t="s">
+        <v>19</v>
+      </c>
+      <c r="E148" t="s">
+        <v>150</v>
+      </c>
+      <c r="F148" t="s">
+        <v>34</v>
+      </c>
+      <c r="G148" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>356</v>
+      </c>
+      <c r="B149" t="s">
+        <v>346</v>
+      </c>
+      <c r="C149" t="s">
+        <v>27</v>
+      </c>
+      <c r="D149" t="s">
+        <v>28</v>
+      </c>
+      <c r="E149" t="s">
+        <v>150</v>
+      </c>
+      <c r="F149" t="s">
+        <v>116</v>
+      </c>
+      <c r="G149" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>357</v>
+      </c>
+      <c r="B150" t="s">
+        <v>348</v>
+      </c>
+      <c r="C150" t="s">
+        <v>27</v>
+      </c>
+      <c r="D150" t="s">
+        <v>28</v>
+      </c>
+      <c r="E150" t="s">
+        <v>150</v>
+      </c>
+      <c r="F150" t="s">
+        <v>116</v>
+      </c>
+      <c r="G150" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>358</v>
+      </c>
+      <c r="B151" t="s">
+        <v>349</v>
+      </c>
+      <c r="C151" t="s">
+        <v>27</v>
+      </c>
+      <c r="D151" t="s">
+        <v>28</v>
+      </c>
+      <c r="E151" t="s">
+        <v>150</v>
+      </c>
+      <c r="F151" t="s">
+        <v>116</v>
+      </c>
+      <c r="G151" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>359</v>
+      </c>
+      <c r="B152" t="s">
+        <v>347</v>
+      </c>
+      <c r="C152" t="s">
+        <v>27</v>
+      </c>
+      <c r="D152" t="s">
+        <v>28</v>
+      </c>
+      <c r="E152" t="s">
+        <v>150</v>
+      </c>
+      <c r="F152" t="s">
+        <v>116</v>
+      </c>
+      <c r="G152" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>360</v>
+      </c>
+      <c r="B153" t="s">
+        <v>350</v>
+      </c>
+      <c r="C153" t="s">
+        <v>27</v>
+      </c>
+      <c r="D153" t="s">
+        <v>28</v>
+      </c>
+      <c r="E153" t="s">
+        <v>150</v>
+      </c>
+      <c r="F153" t="s">
+        <v>116</v>
+      </c>
+      <c r="G153" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>361</v>
+      </c>
+      <c r="B154" t="s">
+        <v>351</v>
+      </c>
+      <c r="C154" t="s">
+        <v>27</v>
+      </c>
+      <c r="D154" t="s">
+        <v>28</v>
+      </c>
+      <c r="E154" t="s">
+        <v>150</v>
+      </c>
+      <c r="F154" t="s">
+        <v>116</v>
+      </c>
+      <c r="G154" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>362</v>
+      </c>
+      <c r="B155" t="s">
+        <v>364</v>
+      </c>
+      <c r="C155" t="s">
+        <v>74</v>
+      </c>
+      <c r="D155" t="s">
+        <v>10</v>
+      </c>
+      <c r="E155" t="s">
+        <v>150</v>
+      </c>
+      <c r="F155" t="s">
+        <v>315</v>
+      </c>
+      <c r="G155" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>363</v>
+      </c>
+      <c r="B156" t="s">
+        <v>365</v>
+      </c>
+      <c r="C156" t="s">
+        <v>74</v>
+      </c>
+      <c r="D156" t="s">
+        <v>10</v>
+      </c>
+      <c r="E156" t="s">
+        <v>150</v>
+      </c>
+      <c r="F156" t="s">
+        <v>315</v>
+      </c>
+      <c r="G156" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>367</v>
+      </c>
+      <c r="B157" t="s">
+        <v>366</v>
+      </c>
+      <c r="C157" t="s">
+        <v>74</v>
+      </c>
+      <c r="D157" t="s">
+        <v>10</v>
+      </c>
+      <c r="E157" t="s">
+        <v>150</v>
+      </c>
+      <c r="F157" t="s">
+        <v>315</v>
+      </c>
+      <c r="G157" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>371</v>
+      </c>
+      <c r="B158" t="s">
+        <v>368</v>
+      </c>
+      <c r="C158" t="s">
+        <v>74</v>
+      </c>
+      <c r="D158" t="s">
+        <v>19</v>
+      </c>
+      <c r="E158" t="s">
+        <v>150</v>
+      </c>
+      <c r="F158" t="s">
+        <v>315</v>
+      </c>
+      <c r="G158" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>373</v>
+      </c>
+      <c r="B159" t="s">
+        <v>369</v>
+      </c>
+      <c r="C159" t="s">
+        <v>74</v>
+      </c>
+      <c r="D159" t="s">
+        <v>19</v>
+      </c>
+      <c r="E159" t="s">
+        <v>150</v>
+      </c>
+      <c r="F159" t="s">
+        <v>315</v>
+      </c>
+      <c r="G159" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>372</v>
+      </c>
+      <c r="B160" t="s">
+        <v>370</v>
+      </c>
+      <c r="C160" t="s">
+        <v>74</v>
+      </c>
+      <c r="D160" t="s">
+        <v>19</v>
+      </c>
+      <c r="E160" t="s">
+        <v>150</v>
+      </c>
+      <c r="F160" t="s">
+        <v>315</v>
+      </c>
+      <c r="G160" t="s">
+        <v>316</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>